<commit_message>
Added ChatApp MAUI data
</commit_message>
<xml_diff>
--- a/data/chatapp-size.xlsx
+++ b/data/chatapp-size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\cross-platform-performance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236DDF77-4D64-4346-9086-9376BCF5BFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B4B4F-CFFF-4B32-ABEB-F777F8E18454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,7 +337,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="0070C0">
+              <a:srgbClr val="7030A0">
                 <a:alpha val="70000"/>
               </a:srgbClr>
             </a:solidFill>
@@ -376,6 +376,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30.7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1405,7 +1408,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,6 +1439,9 @@
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30.7</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated ChatApp size chart
</commit_message>
<xml_diff>
--- a/data/chatapp-size.xlsx
+++ b/data/chatapp-size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\cross-platform-performance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D05EE9-1028-47E0-84CB-ECE19CC78BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1C1800-50E7-4E58-90F7-2C255E84760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,6 +382,9 @@
                 <c:pt idx="2">
                   <c:v>19.600000000000001</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.8</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>46.7</c:v>
                 </c:pt>
@@ -1414,7 +1417,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1470,9 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>29.8</v>
+      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">

</xml_diff>